<commit_message>
Excel Feature: Link Test
</commit_message>
<xml_diff>
--- a/src/test/resources/visitExcelReferenceTest.xlsx
+++ b/src/test/resources/visitExcelReferenceTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Uni\HIWI\metadata_rest_api\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Uni\HIWI\test_version\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EEE3BA-289C-4775-9C36-3785F7F7D421}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1F25D4-C0A7-4B4C-8868-B34A4C482A43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="175">
   <si>
     <t>ID</t>
   </si>
@@ -2000,7 +2000,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2086,8 +2086,8 @@
       <c r="A11" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="144" t="s">
-        <v>81</v>
+      <c r="B11" s="144">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>